<commit_message>
Maj BOM et Workspace
</commit_message>
<xml_diff>
--- a/2-PROJ/14-Carte_Alim_2019/Project Outputs for Carte_Alim_2019/BOM/BOM_Synthetique.xlsx
+++ b/2-PROJ/14-Carte_Alim_2019/Project Outputs for Carte_Alim_2019/BOM/BOM_Synthetique.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Supplier 1 Part Number</t>
   </si>
@@ -22,12 +22,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>1951-3302-ND</t>
-  </si>
-  <si>
-    <t>F4993-ND</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -43,9 +37,6 @@
     <t>CAP CER 100nF 50V X7R 0603</t>
   </si>
   <si>
-    <t>CAP Alu 10'000 UF 25 V</t>
-  </si>
-  <si>
     <t>CAP Alu 330 UF 20% 35 V</t>
   </si>
   <si>
@@ -67,48 +58,15 @@
     <t>DIODE SCHOTTKY 100V 5A SMA (DO-214AC)</t>
   </si>
   <si>
-    <t>Traco 12.0V 60W 5A</t>
-  </si>
-  <si>
-    <t>Traco 5V-6V 30W 6A</t>
-  </si>
-  <si>
-    <t>Traco 5V 15W 3A</t>
-  </si>
-  <si>
-    <t>WE-TVSP Power TVS Diode, Unidirectional, 1500 W, 24 VDC</t>
-  </si>
-  <si>
     <t>FUSE Holder 500V 30A PCB</t>
   </si>
   <si>
-    <t>FUSE AUTO 30A 58VDC BLADE MINI</t>
-  </si>
-  <si>
     <t>Ferrite Bead 180ohm 0603 max1.5A</t>
   </si>
   <si>
-    <t>WR-TBL 2p Series 311 - 5.08 mm Closed Vertical PCB Header</t>
-  </si>
-  <si>
-    <t>WR-MM 6p Female SMT Connector with Polarization</t>
-  </si>
-  <si>
-    <t>picot 2p</t>
-  </si>
-  <si>
-    <t>prise AX-12 3p</t>
-  </si>
-  <si>
-    <t>WR-TBL 2p Series 3221 - 3.50 mm Horizontal PCB Header</t>
-  </si>
-  <si>
     <t>WR-MM 8p Female SMT Connector with Polarization</t>
   </si>
   <si>
-    <t>picot 3p</t>
-  </si>
-  <si>
     <t>WR-TBL 2p Series 3211 - 3.50 mm Vertical PCB Header</t>
   </si>
   <si>
@@ -142,24 +100,9 @@
     <t>RES SMD 68 OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>SWITCH SLIDE SPDT 0.1A 12V (500VDC max)</t>
-  </si>
-  <si>
-    <t>WS-TATV 12x12mm washable Tact Switch, THT version</t>
-  </si>
-  <si>
     <t>Barette seccable 2,54mm 32p</t>
   </si>
   <si>
-    <t>Connecteur fil-à-carte, Libre, 2.54 mm, 6 Contact(s), Mâle, Série WR-MM</t>
-  </si>
-  <si>
-    <t>Connecteur fil-à-carte, Libre, 2.54 mm, 8 Contact(s), Mâle, Série WR-MM</t>
-  </si>
-  <si>
-    <t>Bornier enfichable, 5.08 mm, 2 Voies</t>
-  </si>
-  <si>
     <t>Bornier enfichable, 3,5 mm, 2 Voies</t>
   </si>
   <si>
@@ -170,6 +113,18 @@
   </si>
   <si>
     <t>Patte à braser</t>
+  </si>
+  <si>
+    <t>Micro-Fit 3.0, Embase, 6 Voies</t>
+  </si>
+  <si>
+    <t>Contact, RMF™, Série Micro-Fit 3.0 AWG26</t>
+  </si>
+  <si>
+    <t>Mini-Fit Jr. Série, Embase, 4 Voies</t>
+  </si>
+  <si>
+    <t>Contact, Mini-Fit® Jr.™, Série 5556, AWG18</t>
   </si>
 </sst>
 </file>
@@ -220,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -231,6 +186,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -564,7 +523,7 @@
         <v>60</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -575,7 +534,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -586,7 +545,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -597,491 +556,337 @@
         <v>100</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>2465697</v>
+        <v>2465709</v>
       </c>
       <c r="B6" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>2465709</v>
+        <v>2533610</v>
       </c>
       <c r="B7" s="3">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>2533610</v>
+        <v>2495167</v>
       </c>
       <c r="B8" s="3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>2495167</v>
+        <v>2322070</v>
       </c>
       <c r="B9" s="3">
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>2322070</v>
+        <v>2581593</v>
       </c>
       <c r="B10" s="3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>2581593</v>
+        <v>9526510</v>
       </c>
       <c r="B11" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>9526510</v>
+        <v>2750942</v>
       </c>
       <c r="B12" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>2750942</v>
+        <v>2292904</v>
       </c>
       <c r="B13" s="3">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>2451635</v>
+        <v>1800355</v>
       </c>
       <c r="B14" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
+      <c r="A15" s="1">
+        <v>1641850</v>
       </c>
       <c r="B15" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>1441226</v>
+        <v>1841308</v>
       </c>
       <c r="B16" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>2839627</v>
+        <v>2443434</v>
       </c>
       <c r="B17" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>2292904</v>
+        <v>1831088</v>
       </c>
       <c r="B18" s="3">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>3</v>
+      <c r="A19" s="1">
+        <v>2762691</v>
       </c>
       <c r="B19" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>1800355</v>
+        <v>9238603</v>
       </c>
       <c r="B20" s="3">
-        <v>24</v>
+        <v>270</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>1641978</v>
+        <v>1903754</v>
       </c>
       <c r="B21" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>1641849</v>
+        <v>9237666</v>
       </c>
       <c r="B22" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>9731075</v>
+        <v>9238484</v>
       </c>
       <c r="B23" s="3">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>9979620</v>
+        <v>9238514</v>
       </c>
       <c r="B24" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>1841315</v>
+        <v>1458815</v>
       </c>
       <c r="B25" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>1641850</v>
+        <v>9238344</v>
       </c>
       <c r="B26" s="3">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>9731083</v>
+        <v>1022263</v>
       </c>
       <c r="B27" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>1841308</v>
+        <v>672907</v>
       </c>
       <c r="B28" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>2443434</v>
+        <v>2063718</v>
       </c>
       <c r="B29" s="3">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>1831088</v>
+        <v>151867</v>
       </c>
       <c r="B30" s="3">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>2762691</v>
+        <v>1462545</v>
       </c>
       <c r="B31" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>9238603</v>
+        <v>1841347</v>
       </c>
       <c r="B32" s="3">
-        <v>270</v>
+        <v>7</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>1903754</v>
+      <c r="A33" s="4">
+        <v>2137132</v>
       </c>
       <c r="B33" s="3">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>36</v>
+        <v>10</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>9237666</v>
+      <c r="A34" s="4">
+        <v>2137134</v>
       </c>
       <c r="B34" s="3">
-        <v>20</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>9238484</v>
+      <c r="A35" s="4">
+        <v>1850223</v>
       </c>
       <c r="B35" s="3">
-        <v>110</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>9238514</v>
-      </c>
-      <c r="B36" s="3">
-        <v>20</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>1458815</v>
-      </c>
-      <c r="B37" s="3">
-        <v>10</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>9238344</v>
-      </c>
-      <c r="B38" s="3">
-        <v>40</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>1201430</v>
-      </c>
-      <c r="B39" s="3">
-        <v>0</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>2065140</v>
-      </c>
-      <c r="B40" s="3">
-        <v>0</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>1022263</v>
-      </c>
-      <c r="B41" s="3">
-        <v>6</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>1641882</v>
-      </c>
-      <c r="B42" s="3">
-        <v>0</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>1641883</v>
-      </c>
-      <c r="B43" s="3">
-        <v>5</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
-        <v>1641952</v>
-      </c>
-      <c r="B44" s="3">
-        <v>0</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
-        <v>1841347</v>
-      </c>
-      <c r="B45" s="3">
-        <v>10</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>2137132</v>
-      </c>
-      <c r="B46" s="3">
-        <v>10</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
-        <v>2137134</v>
-      </c>
-      <c r="B47" s="3">
-        <v>10</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>1850223</v>
-      </c>
-      <c r="B48" s="3">
         <v>1</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>2065138</v>
-      </c>
-      <c r="B49" s="3">
-        <v>0</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>43</v>
+      <c r="C35" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>